<commit_message>
updated integ fix errors
</commit_message>
<xml_diff>
--- a/src/Backend/Integration/batchresults.xlsx
+++ b/src/Backend/Integration/batchresults.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaynb\Documents\COMP0016-Team-3\src\Backend\Integration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF958B4F-7DD2-4A0E-B3A3-216F363D7882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>path</t>
   </si>
@@ -58,47 +64,122 @@
     <t>src/Backend/Integration/MDRRW014dfr.pdf</t>
   </si>
   <si>
+    <t>sampledocs\MDRUG040efr.pdf</t>
+  </si>
+  <si>
+    <t>sampledocs/MDRJM004dfr.pdf</t>
+  </si>
+  <si>
     <t>Rwanda</t>
   </si>
   <si>
+    <t>Democratic Republic 
+of Congo</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
     <t>RWA</t>
   </si>
   <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>HAI</t>
+  </si>
+  <si>
     <t xml:space="preserve">20RWA001 </t>
   </si>
   <si>
+    <t xml:space="preserve">20COD903 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">20R053WA005053 </t>
   </si>
   <si>
+    <t xml:space="preserve">20COD502010 </t>
+  </si>
+  <si>
     <t>11 July 2017</t>
   </si>
   <si>
+    <t>17 January 2018</t>
+  </si>
+  <si>
+    <t>1 October 2016</t>
+  </si>
+  <si>
     <t>01 September 2017</t>
   </si>
   <si>
-    <t>675</t>
+    <t>31 December 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+DREF Operation Final Report</t>
+  </si>
+  <si>
+    <t>48,500</t>
+  </si>
+  <si>
+    <t>100,000 to  
+150,000 persons</t>
   </si>
   <si>
     <t>811 households</t>
   </si>
   <si>
+    <t>18,000</t>
+  </si>
+  <si>
+    <t>524 families</t>
+  </si>
+  <si>
     <t>ST-2017 -000035 -RWA</t>
   </si>
   <si>
+    <t>EP-2018 -000021 -UGA</t>
+  </si>
+  <si>
+    <t>Category 5</t>
+  </si>
+  <si>
     <t>MDRRW014</t>
   </si>
   <si>
+    <t>Emergency Appeal</t>
+  </si>
+  <si>
+    <t>MDRJM004</t>
+  </si>
+  <si>
     <t>CHF 49,122</t>
   </si>
   <si>
+    <t>CHF 3,200,000</t>
+  </si>
+  <si>
+    <t>130,149 Swiss francs</t>
+  </si>
+  <si>
     <t>Rwanda Red Cross Society</t>
+  </si>
+  <si>
+    <t>Uganda Red Cross Society</t>
+  </si>
+  <si>
+    <t>The Jamaica Red Cross</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +242,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -207,7 +296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,9 +328,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -273,6 +380,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -448,14 +573,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="4" max="4" width="15.68359375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,127 +624,127 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H2">
         <v>675</v>
       </c>
       <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3">
-        <v>675</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>